<commit_message>
Tidy up HawksBay2013 a bit
</commit_message>
<xml_diff>
--- a/Prototypes/Maize/Observations/LeafSenesCount.xlsx
+++ b/Prototypes/Maize/Observations/LeafSenesCount.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="22980" windowHeight="9000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="22980" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="StartSenes" sheetId="1" r:id="rId1"/>
@@ -108,31 +108,13 @@
     <t>Dry_000N</t>
   </si>
   <si>
-    <t>Lincoln2012NitrogenNilIrrigationNil</t>
-  </si>
-  <si>
     <t>Dry_075N</t>
-  </si>
-  <si>
-    <t>Lincoln2012NitrogenLowIrrigationNil</t>
-  </si>
-  <si>
-    <t>Lincoln2012NitrogenMedIrrigationNil</t>
   </si>
   <si>
     <t>Irrig_000N</t>
   </si>
   <si>
-    <t>Lincoln2012NitrogenNilIrrigationFull</t>
-  </si>
-  <si>
     <t>Irrig_075N</t>
-  </si>
-  <si>
-    <t>Lincoln2012NitrogenLowIrrigationFull</t>
-  </si>
-  <si>
-    <t>Lincoln2012NitrogenMedIrrigationFull</t>
   </si>
   <si>
     <t>000N</t>
@@ -157,6 +139,24 @@
   </si>
   <si>
     <t>Nitro</t>
+  </si>
+  <si>
+    <t>Lincoln2012NitNilIrrNil</t>
+  </si>
+  <si>
+    <t>Lincoln2012NitLowIrrNil</t>
+  </si>
+  <si>
+    <t>Lincoln2012NitMedIrrNil</t>
+  </si>
+  <si>
+    <t>Lincoln2012NitNilIrrFull</t>
+  </si>
+  <si>
+    <t>Lincoln2012NitLowIrrFull</t>
+  </si>
+  <si>
+    <t>Lincoln2012NitMedIrrFull</t>
   </si>
 </sst>
 </file>
@@ -507,41 +507,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="str">
         <f>VLOOKUP(B2,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -550,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1">
         <v>41261.666666666664</v>
@@ -562,7 +562,7 @@
     <row r="3" spans="1:6">
       <c r="A3" t="str">
         <f>VLOOKUP(B3,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -571,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>41263.625</v>
@@ -583,7 +583,7 @@
     <row r="4" spans="1:6">
       <c r="A4" t="str">
         <f>VLOOKUP(B4,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -592,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>41269.75</v>
@@ -604,7 +604,7 @@
     <row r="5" spans="1:6">
       <c r="A5" t="str">
         <f>VLOOKUP(B5,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>41270.5</v>
@@ -625,7 +625,7 @@
     <row r="6" spans="1:6">
       <c r="A6" t="str">
         <f>VLOOKUP(B6,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1">
         <v>41276.166666666664</v>
@@ -646,7 +646,7 @@
     <row r="7" spans="1:6">
       <c r="A7" t="str">
         <f>VLOOKUP(B7,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -655,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <v>41277</v>
@@ -667,7 +667,7 @@
     <row r="8" spans="1:6">
       <c r="A8" t="str">
         <f>VLOOKUP(B8,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1">
         <v>41278.041666666664</v>
@@ -688,7 +688,7 @@
     <row r="9" spans="1:6">
       <c r="A9" t="str">
         <f>VLOOKUP(B9,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1">
         <v>41283.625</v>
@@ -709,7 +709,7 @@
     <row r="10" spans="1:6">
       <c r="A10" t="str">
         <f>VLOOKUP(B10,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1">
         <v>41284.75</v>
@@ -730,7 +730,7 @@
     <row r="11" spans="1:6">
       <c r="A11" t="str">
         <f>VLOOKUP(B11,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1">
         <v>41292.375000000007</v>
@@ -751,7 +751,7 @@
     <row r="12" spans="1:6">
       <c r="A12" t="str">
         <f>VLOOKUP(B12,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -760,7 +760,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1">
         <v>41298.791666666664</v>
@@ -772,7 +772,7 @@
     <row r="13" spans="1:6">
       <c r="A13" t="str">
         <f>VLOOKUP(B13,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1">
         <v>41306.875</v>
@@ -793,7 +793,7 @@
     <row r="14" spans="1:6">
       <c r="A14" t="str">
         <f>VLOOKUP(B14,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -802,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <v>41318.083333333336</v>
@@ -814,7 +814,7 @@
     <row r="15" spans="1:6">
       <c r="A15" t="str">
         <f>VLOOKUP(B15,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -823,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1">
         <v>41333.583333333336</v>
@@ -835,7 +835,7 @@
     <row r="16" spans="1:6">
       <c r="A16" t="str">
         <f>VLOOKUP(B16,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1">
         <v>41342.183333333334</v>
@@ -856,7 +856,7 @@
     <row r="17" spans="1:6">
       <c r="A17" t="str">
         <f>VLOOKUP(B17,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1">
         <v>41342.791666666664</v>
@@ -877,7 +877,7 @@
     <row r="18" spans="1:6">
       <c r="A18" t="str">
         <f>VLOOKUP(B18,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -886,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1">
         <v>41345.050000000003</v>
@@ -898,16 +898,16 @@
     <row r="19" spans="1:6">
       <c r="A19" t="str">
         <f>VLOOKUP(B19,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1">
         <v>41261.916666666672</v>
@@ -919,16 +919,16 @@
     <row r="20" spans="1:6">
       <c r="A20" t="str">
         <f>VLOOKUP(B20,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E20" s="1">
         <v>41265.416666666672</v>
@@ -940,16 +940,16 @@
     <row r="21" spans="1:6">
       <c r="A21" t="str">
         <f>VLOOKUP(B21,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1">
         <v>41269.875</v>
@@ -961,16 +961,16 @@
     <row r="22" spans="1:6">
       <c r="A22" t="str">
         <f>VLOOKUP(B22,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1">
         <v>41271.875</v>
@@ -982,16 +982,16 @@
     <row r="23" spans="1:6">
       <c r="A23" t="str">
         <f>VLOOKUP(B23,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1">
         <v>41277</v>
@@ -1003,16 +1003,16 @@
     <row r="24" spans="1:6">
       <c r="A24" t="str">
         <f>VLOOKUP(B24,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1">
         <v>41278.5</v>
@@ -1024,16 +1024,16 @@
     <row r="25" spans="1:6">
       <c r="A25" t="str">
         <f>VLOOKUP(B25,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1">
         <v>41281</v>
@@ -1045,16 +1045,16 @@
     <row r="26" spans="1:6">
       <c r="A26" t="str">
         <f>VLOOKUP(B26,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1">
         <v>41284.75</v>
@@ -1066,16 +1066,16 @@
     <row r="27" spans="1:6">
       <c r="A27" t="str">
         <f>VLOOKUP(B27,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E27" s="1">
         <v>41289.041666666664</v>
@@ -1087,16 +1087,16 @@
     <row r="28" spans="1:6">
       <c r="A28" t="str">
         <f>VLOOKUP(B28,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E28" s="1">
         <v>41295.041666666672</v>
@@ -1108,16 +1108,16 @@
     <row r="29" spans="1:6">
       <c r="A29" t="str">
         <f>VLOOKUP(B29,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E29" s="1">
         <v>41299.458333333336</v>
@@ -1129,16 +1129,16 @@
     <row r="30" spans="1:6">
       <c r="A30" t="str">
         <f>VLOOKUP(B30,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E30" s="1">
         <v>41304.041666666672</v>
@@ -1150,16 +1150,16 @@
     <row r="31" spans="1:6">
       <c r="A31" t="str">
         <f>VLOOKUP(B31,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1">
         <v>41316.125</v>
@@ -1171,16 +1171,16 @@
     <row r="32" spans="1:6">
       <c r="A32" t="str">
         <f>VLOOKUP(B32,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1">
         <v>41328.499999999993</v>
@@ -1192,16 +1192,16 @@
     <row r="33" spans="1:6">
       <c r="A33" t="str">
         <f>VLOOKUP(B33,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E33" s="1">
         <v>41337.583333333336</v>
@@ -1213,16 +1213,16 @@
     <row r="34" spans="1:6">
       <c r="A34" t="str">
         <f>VLOOKUP(B34,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1">
         <v>41338.666666666664</v>
@@ -1234,16 +1234,16 @@
     <row r="35" spans="1:6">
       <c r="A35" t="str">
         <f>VLOOKUP(B35,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E35" s="1">
         <v>41339.25</v>
@@ -1255,16 +1255,16 @@
     <row r="36" spans="1:6">
       <c r="A36" t="str">
         <f>VLOOKUP(B36,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1">
         <v>41353</v>
@@ -1276,7 +1276,7 @@
     <row r="37" spans="1:6">
       <c r="A37" t="str">
         <f>VLOOKUP(B37,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -1297,7 +1297,7 @@
     <row r="38" spans="1:6">
       <c r="A38" t="str">
         <f>VLOOKUP(B38,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -1318,7 +1318,7 @@
     <row r="39" spans="1:6">
       <c r="A39" t="str">
         <f>VLOOKUP(B39,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -1339,7 +1339,7 @@
     <row r="40" spans="1:6">
       <c r="A40" t="str">
         <f>VLOOKUP(B40,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
@@ -1360,7 +1360,7 @@
     <row r="41" spans="1:6">
       <c r="A41" t="str">
         <f>VLOOKUP(B41,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -1381,7 +1381,7 @@
     <row r="42" spans="1:6">
       <c r="A42" t="str">
         <f>VLOOKUP(B42,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -1402,7 +1402,7 @@
     <row r="43" spans="1:6">
       <c r="A43" t="str">
         <f>VLOOKUP(B43,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
@@ -1423,7 +1423,7 @@
     <row r="44" spans="1:6">
       <c r="A44" t="str">
         <f>VLOOKUP(B44,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -1444,7 +1444,7 @@
     <row r="45" spans="1:6">
       <c r="A45" t="str">
         <f>VLOOKUP(B45,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -1465,7 +1465,7 @@
     <row r="46" spans="1:6">
       <c r="A46" t="str">
         <f>VLOOKUP(B46,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -1486,7 +1486,7 @@
     <row r="47" spans="1:6">
       <c r="A47" t="str">
         <f>VLOOKUP(B47,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -1507,7 +1507,7 @@
     <row r="48" spans="1:6">
       <c r="A48" t="str">
         <f>VLOOKUP(B48,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -1528,7 +1528,7 @@
     <row r="49" spans="1:6">
       <c r="A49" t="str">
         <f>VLOOKUP(B49,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -1549,7 +1549,7 @@
     <row r="50" spans="1:6">
       <c r="A50" t="str">
         <f>VLOOKUP(B50,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -1570,7 +1570,7 @@
     <row r="51" spans="1:6">
       <c r="A51" t="str">
         <f>VLOOKUP(B51,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -1591,7 +1591,7 @@
     <row r="52" spans="1:6">
       <c r="A52" t="str">
         <f>VLOOKUP(B52,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
@@ -1612,7 +1612,7 @@
     <row r="53" spans="1:6">
       <c r="A53" t="str">
         <f>VLOOKUP(B53,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
@@ -1633,16 +1633,16 @@
     <row r="54" spans="1:6">
       <c r="A54" t="str">
         <f>VLOOKUP(B54,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E54" s="1">
         <v>41263.666666666672</v>
@@ -1654,16 +1654,16 @@
     <row r="55" spans="1:6">
       <c r="A55" t="str">
         <f>VLOOKUP(B55,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E55" s="1">
         <v>41268.125</v>
@@ -1675,16 +1675,16 @@
     <row r="56" spans="1:6">
       <c r="A56" t="str">
         <f>VLOOKUP(B56,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1">
         <v>41271.583333333328</v>
@@ -1696,16 +1696,16 @@
     <row r="57" spans="1:6">
       <c r="A57" t="str">
         <f>VLOOKUP(B57,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1">
         <v>41276.75</v>
@@ -1717,16 +1717,16 @@
     <row r="58" spans="1:6">
       <c r="A58" t="str">
         <f>VLOOKUP(B58,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E58" s="1">
         <v>41279.75</v>
@@ -1738,16 +1738,16 @@
     <row r="59" spans="1:6">
       <c r="A59" t="str">
         <f>VLOOKUP(B59,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E59" s="1">
         <v>41282.25</v>
@@ -1759,16 +1759,16 @@
     <row r="60" spans="1:6">
       <c r="A60" t="str">
         <f>VLOOKUP(B60,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E60" s="1">
         <v>41285.041666666664</v>
@@ -1780,16 +1780,16 @@
     <row r="61" spans="1:6">
       <c r="A61" t="str">
         <f>VLOOKUP(B61,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E61" s="1">
         <v>41291.083333333328</v>
@@ -1801,16 +1801,16 @@
     <row r="62" spans="1:6">
       <c r="A62" t="str">
         <f>VLOOKUP(B62,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E62" s="1">
         <v>41306.875000000007</v>
@@ -1822,16 +1822,16 @@
     <row r="63" spans="1:6">
       <c r="A63" t="str">
         <f>VLOOKUP(B63,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E63" s="1">
         <v>41338</v>
@@ -1843,16 +1843,16 @@
     <row r="64" spans="1:6">
       <c r="A64" t="str">
         <f>VLOOKUP(B64,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E64" s="1">
         <v>41347.583333333336</v>
@@ -1864,16 +1864,16 @@
     <row r="65" spans="1:6">
       <c r="A65" t="str">
         <f>VLOOKUP(B65,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1">
         <v>41348.566666666666</v>
@@ -1885,16 +1885,16 @@
     <row r="66" spans="1:6">
       <c r="A66" t="str">
         <f>VLOOKUP(B66,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E66" s="1">
         <v>41353.35</v>
@@ -1906,16 +1906,16 @@
     <row r="67" spans="1:6">
       <c r="A67" t="str">
         <f>VLOOKUP(B67,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E67" s="1">
         <v>41354.408333333333</v>
@@ -1927,16 +1927,16 @@
     <row r="68" spans="1:6">
       <c r="A68" t="str">
         <f>VLOOKUP(B68,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E68" s="1">
         <v>41355.444444444445</v>
@@ -1948,16 +1948,16 @@
     <row r="69" spans="1:6">
       <c r="A69" t="str">
         <f>VLOOKUP(B69,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E69" s="1">
         <v>41356.066666666666</v>
@@ -1969,16 +1969,16 @@
     <row r="70" spans="1:6">
       <c r="A70" t="str">
         <f>VLOOKUP(B70,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E70" s="1">
         <v>41358.25</v>
@@ -1990,16 +1990,16 @@
     <row r="71" spans="1:6">
       <c r="A71" t="str">
         <f>VLOOKUP(B71,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E71" s="1">
         <v>41265.25</v>
@@ -2011,16 +2011,16 @@
     <row r="72" spans="1:6">
       <c r="A72" t="str">
         <f>VLOOKUP(B72,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E72" s="1">
         <v>41271.041666666672</v>
@@ -2032,16 +2032,16 @@
     <row r="73" spans="1:6">
       <c r="A73" t="str">
         <f>VLOOKUP(B73,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E73" s="1">
         <v>41278.708333333336</v>
@@ -2053,16 +2053,16 @@
     <row r="74" spans="1:6">
       <c r="A74" t="str">
         <f>VLOOKUP(B74,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E74" s="1">
         <v>41282.625</v>
@@ -2074,16 +2074,16 @@
     <row r="75" spans="1:6">
       <c r="A75" t="str">
         <f>VLOOKUP(B75,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E75" s="1">
         <v>41286.833333333336</v>
@@ -2095,16 +2095,16 @@
     <row r="76" spans="1:6">
       <c r="A76" t="str">
         <f>VLOOKUP(B76,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E76" s="1">
         <v>41289.208333333328</v>
@@ -2116,16 +2116,16 @@
     <row r="77" spans="1:6">
       <c r="A77" t="str">
         <f>VLOOKUP(B77,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E77" s="1">
         <v>41294.333333333336</v>
@@ -2137,16 +2137,16 @@
     <row r="78" spans="1:6">
       <c r="A78" t="str">
         <f>VLOOKUP(B78,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E78" s="1">
         <v>41305.041666666672</v>
@@ -2158,16 +2158,16 @@
     <row r="79" spans="1:6">
       <c r="A79" t="str">
         <f>VLOOKUP(B79,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E79" s="1">
         <v>41327.791666666664</v>
@@ -2179,16 +2179,16 @@
     <row r="80" spans="1:6">
       <c r="A80" t="str">
         <f>VLOOKUP(B80,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E80" s="1">
         <v>41350.008333333331</v>
@@ -2200,16 +2200,16 @@
     <row r="81" spans="1:6">
       <c r="A81" t="str">
         <f>VLOOKUP(B81,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C81" t="s">
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E81" s="1">
         <v>41356</v>
@@ -2221,16 +2221,16 @@
     <row r="82" spans="1:6">
       <c r="A82" t="str">
         <f>VLOOKUP(B82,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B82" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C82" t="s">
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E82" s="1">
         <v>41357.944444444445</v>
@@ -2242,16 +2242,16 @@
     <row r="83" spans="1:6">
       <c r="A83" t="str">
         <f>VLOOKUP(B83,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E83" s="1">
         <v>41359</v>
@@ -2263,7 +2263,7 @@
     <row r="84" spans="1:6">
       <c r="A84" t="str">
         <f>VLOOKUP(B84,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B84" t="s">
         <v>4</v>
@@ -2284,7 +2284,7 @@
     <row r="85" spans="1:6">
       <c r="A85" t="str">
         <f>VLOOKUP(B85,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B85" t="s">
         <v>4</v>
@@ -2305,7 +2305,7 @@
     <row r="86" spans="1:6">
       <c r="A86" t="str">
         <f>VLOOKUP(B86,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B86" t="s">
         <v>4</v>
@@ -2326,7 +2326,7 @@
     <row r="87" spans="1:6">
       <c r="A87" t="str">
         <f>VLOOKUP(B87,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B87" t="s">
         <v>4</v>
@@ -2347,7 +2347,7 @@
     <row r="88" spans="1:6">
       <c r="A88" t="str">
         <f>VLOOKUP(B88,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B88" t="s">
         <v>4</v>
@@ -2368,7 +2368,7 @@
     <row r="89" spans="1:6">
       <c r="A89" t="str">
         <f>VLOOKUP(B89,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B89" t="s">
         <v>4</v>
@@ -2389,7 +2389,7 @@
     <row r="90" spans="1:6">
       <c r="A90" t="str">
         <f>VLOOKUP(B90,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B90" t="s">
         <v>4</v>
@@ -2410,7 +2410,7 @@
     <row r="91" spans="1:6">
       <c r="A91" t="str">
         <f>VLOOKUP(B91,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B91" t="s">
         <v>4</v>
@@ -2431,7 +2431,7 @@
     <row r="92" spans="1:6">
       <c r="A92" t="str">
         <f>VLOOKUP(B92,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B92" t="s">
         <v>4</v>
@@ -2452,7 +2452,7 @@
     <row r="93" spans="1:6">
       <c r="A93" t="str">
         <f>VLOOKUP(B93,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B93" t="s">
         <v>4</v>
@@ -2473,7 +2473,7 @@
     <row r="94" spans="1:6">
       <c r="A94" t="str">
         <f>VLOOKUP(B94,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B94" t="s">
         <v>4</v>
@@ -2494,7 +2494,7 @@
     <row r="95" spans="1:6">
       <c r="A95" t="str">
         <f>VLOOKUP(B95,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B95" t="s">
         <v>4</v>
@@ -2523,47 +2523,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="str">
         <f>VLOOKUP(B2,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -2572,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1">
         <v>41270</v>
@@ -2584,7 +2584,7 @@
     <row r="3" spans="1:7">
       <c r="A3" t="str">
         <f>VLOOKUP(B3,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>41270.875</v>
@@ -2605,7 +2605,7 @@
     <row r="4" spans="1:7">
       <c r="A4" t="str">
         <f>VLOOKUP(B4,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -2614,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>41276.708333333336</v>
@@ -2626,7 +2626,7 @@
     <row r="5" spans="1:7">
       <c r="A5" t="str">
         <f>VLOOKUP(B5,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -2635,7 +2635,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>41277</v>
@@ -2647,7 +2647,7 @@
     <row r="6" spans="1:7">
       <c r="A6" t="str">
         <f>VLOOKUP(B6,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -2656,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1">
         <v>41282.5</v>
@@ -2668,7 +2668,7 @@
     <row r="7" spans="1:7">
       <c r="A7" t="str">
         <f>VLOOKUP(B7,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -2677,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <v>41289.708333333336</v>
@@ -2689,7 +2689,7 @@
     <row r="8" spans="1:7">
       <c r="A8" t="str">
         <f>VLOOKUP(B8,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -2698,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1">
         <v>41298</v>
@@ -2710,7 +2710,7 @@
     <row r="9" spans="1:7">
       <c r="A9" t="str">
         <f>VLOOKUP(B9,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -2719,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1">
         <v>41304.916666666672</v>
@@ -2731,7 +2731,7 @@
     <row r="10" spans="1:7">
       <c r="A10" t="str">
         <f>VLOOKUP(B10,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1">
         <v>41312.125</v>
@@ -2752,7 +2752,7 @@
     <row r="11" spans="1:7">
       <c r="A11" t="str">
         <f>VLOOKUP(B11,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -2761,7 +2761,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1">
         <v>41342.216666666667</v>
@@ -2773,7 +2773,7 @@
     <row r="12" spans="1:7">
       <c r="A12" t="str">
         <f>VLOOKUP(B12,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -2782,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1">
         <v>41358.5</v>
@@ -2794,7 +2794,7 @@
     <row r="13" spans="1:7">
       <c r="A13" t="str">
         <f>VLOOKUP(B13,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -2803,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1">
         <v>41359</v>
@@ -2815,7 +2815,7 @@
     <row r="14" spans="1:7">
       <c r="A14" t="str">
         <f>VLOOKUP(B14,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -2824,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <v>41359</v>
@@ -2836,7 +2836,7 @@
     <row r="15" spans="1:7">
       <c r="A15" t="str">
         <f>VLOOKUP(B15,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -2845,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1">
         <v>41359</v>
@@ -2857,7 +2857,7 @@
     <row r="16" spans="1:7">
       <c r="A16" t="str">
         <f>VLOOKUP(B16,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -2866,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1">
         <v>41359</v>
@@ -2878,7 +2878,7 @@
     <row r="17" spans="1:6">
       <c r="A17" t="str">
         <f>VLOOKUP(B17,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationNil</v>
+        <v>Lincoln2012NitNilIrrNil</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1">
         <v>41357.525000000001</v>
@@ -2899,16 +2899,16 @@
     <row r="18" spans="1:6">
       <c r="A18" t="str">
         <f>VLOOKUP(B18,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1">
         <v>41270.208333333336</v>
@@ -2920,16 +2920,16 @@
     <row r="19" spans="1:6">
       <c r="A19" t="str">
         <f>VLOOKUP(B19,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1">
         <v>41272.916666666664</v>
@@ -2941,16 +2941,16 @@
     <row r="20" spans="1:6">
       <c r="A20" t="str">
         <f>VLOOKUP(B20,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E20" s="1">
         <v>41276.708333333336</v>
@@ -2962,16 +2962,16 @@
     <row r="21" spans="1:6">
       <c r="A21" t="str">
         <f>VLOOKUP(B21,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1">
         <v>41278</v>
@@ -2983,16 +2983,16 @@
     <row r="22" spans="1:6">
       <c r="A22" t="str">
         <f>VLOOKUP(B22,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1">
         <v>41284.458333333336</v>
@@ -3004,16 +3004,16 @@
     <row r="23" spans="1:6">
       <c r="A23" t="str">
         <f>VLOOKUP(B23,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1">
         <v>41291</v>
@@ -3025,16 +3025,16 @@
     <row r="24" spans="1:6">
       <c r="A24" t="str">
         <f>VLOOKUP(B24,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1">
         <v>41297.625</v>
@@ -3046,16 +3046,16 @@
     <row r="25" spans="1:6">
       <c r="A25" t="str">
         <f>VLOOKUP(B25,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1">
         <v>41305.5</v>
@@ -3067,16 +3067,16 @@
     <row r="26" spans="1:6">
       <c r="A26" t="str">
         <f>VLOOKUP(B26,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1">
         <v>41318.500000000007</v>
@@ -3088,16 +3088,16 @@
     <row r="27" spans="1:6">
       <c r="A27" t="str">
         <f>VLOOKUP(B27,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E27" s="1">
         <v>41343.258333333331</v>
@@ -3109,16 +3109,16 @@
     <row r="28" spans="1:6">
       <c r="A28" t="str">
         <f>VLOOKUP(B28,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E28" s="1">
         <v>41356.208333333336</v>
@@ -3130,16 +3130,16 @@
     <row r="29" spans="1:6">
       <c r="A29" t="str">
         <f>VLOOKUP(B29,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E29" s="1">
         <v>41359</v>
@@ -3151,16 +3151,16 @@
     <row r="30" spans="1:6">
       <c r="A30" t="str">
         <f>VLOOKUP(B30,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E30" s="1">
         <v>41359</v>
@@ -3172,16 +3172,16 @@
     <row r="31" spans="1:6">
       <c r="A31" t="str">
         <f>VLOOKUP(B31,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1">
         <v>41359</v>
@@ -3193,16 +3193,16 @@
     <row r="32" spans="1:6">
       <c r="A32" t="str">
         <f>VLOOKUP(B32,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1">
         <v>41359</v>
@@ -3214,16 +3214,16 @@
     <row r="33" spans="1:6">
       <c r="A33" t="str">
         <f>VLOOKUP(B33,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E33" s="1">
         <v>41358.625</v>
@@ -3235,16 +3235,16 @@
     <row r="34" spans="1:6">
       <c r="A34" t="str">
         <f>VLOOKUP(B34,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1">
         <v>41353.51666666667</v>
@@ -3256,16 +3256,16 @@
     <row r="35" spans="1:6">
       <c r="A35" t="str">
         <f>VLOOKUP(B35,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E35" s="1">
         <v>41359</v>
@@ -3277,16 +3277,16 @@
     <row r="36" spans="1:6">
       <c r="A36" t="str">
         <f>VLOOKUP(B36,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationNil</v>
+        <v>Lincoln2012NitLowIrrNil</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1">
         <v>41359</v>
@@ -3298,7 +3298,7 @@
     <row r="37" spans="1:6">
       <c r="A37" t="str">
         <f>VLOOKUP(B37,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -3319,7 +3319,7 @@
     <row r="38" spans="1:6">
       <c r="A38" t="str">
         <f>VLOOKUP(B38,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
@@ -3340,7 +3340,7 @@
     <row r="39" spans="1:6">
       <c r="A39" t="str">
         <f>VLOOKUP(B39,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -3361,7 +3361,7 @@
     <row r="40" spans="1:6">
       <c r="A40" t="str">
         <f>VLOOKUP(B40,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
@@ -3382,7 +3382,7 @@
     <row r="41" spans="1:6">
       <c r="A41" t="str">
         <f>VLOOKUP(B41,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -3403,7 +3403,7 @@
     <row r="42" spans="1:6">
       <c r="A42" t="str">
         <f>VLOOKUP(B42,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -3424,7 +3424,7 @@
     <row r="43" spans="1:6">
       <c r="A43" t="str">
         <f>VLOOKUP(B43,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
@@ -3445,7 +3445,7 @@
     <row r="44" spans="1:6">
       <c r="A44" t="str">
         <f>VLOOKUP(B44,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
@@ -3466,7 +3466,7 @@
     <row r="45" spans="1:6">
       <c r="A45" t="str">
         <f>VLOOKUP(B45,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B45" t="s">
         <v>1</v>
@@ -3487,7 +3487,7 @@
     <row r="46" spans="1:6">
       <c r="A46" t="str">
         <f>VLOOKUP(B46,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -3508,7 +3508,7 @@
     <row r="47" spans="1:6">
       <c r="A47" t="str">
         <f>VLOOKUP(B47,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B47" t="s">
         <v>1</v>
@@ -3529,7 +3529,7 @@
     <row r="48" spans="1:6">
       <c r="A48" t="str">
         <f>VLOOKUP(B48,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -3550,7 +3550,7 @@
     <row r="49" spans="1:6">
       <c r="A49" t="str">
         <f>VLOOKUP(B49,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B49" t="s">
         <v>1</v>
@@ -3571,7 +3571,7 @@
     <row r="50" spans="1:6">
       <c r="A50" t="str">
         <f>VLOOKUP(B50,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -3592,7 +3592,7 @@
     <row r="51" spans="1:6">
       <c r="A51" t="str">
         <f>VLOOKUP(B51,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
@@ -3613,7 +3613,7 @@
     <row r="52" spans="1:6">
       <c r="A52" t="str">
         <f>VLOOKUP(B52,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B52" t="s">
         <v>1</v>
@@ -3634,7 +3634,7 @@
     <row r="53" spans="1:6">
       <c r="A53" t="str">
         <f>VLOOKUP(B53,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationNil</v>
+        <v>Lincoln2012NitMedIrrNil</v>
       </c>
       <c r="B53" t="s">
         <v>1</v>
@@ -3655,16 +3655,16 @@
     <row r="54" spans="1:6">
       <c r="A54" t="str">
         <f>VLOOKUP(B54,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E54" s="1">
         <v>41272.333333333336</v>
@@ -3676,16 +3676,16 @@
     <row r="55" spans="1:6">
       <c r="A55" t="str">
         <f>VLOOKUP(B55,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E55" s="1">
         <v>41275.541666666664</v>
@@ -3697,16 +3697,16 @@
     <row r="56" spans="1:6">
       <c r="A56" t="str">
         <f>VLOOKUP(B56,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1">
         <v>41278.75</v>
@@ -3718,16 +3718,16 @@
     <row r="57" spans="1:6">
       <c r="A57" t="str">
         <f>VLOOKUP(B57,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1">
         <v>41283.041666666664</v>
@@ -3739,16 +3739,16 @@
     <row r="58" spans="1:6">
       <c r="A58" t="str">
         <f>VLOOKUP(B58,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E58" s="1">
         <v>41290.416666666664</v>
@@ -3760,16 +3760,16 @@
     <row r="59" spans="1:6">
       <c r="A59" t="str">
         <f>VLOOKUP(B59,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E59" s="1">
         <v>41293.333333333328</v>
@@ -3781,16 +3781,16 @@
     <row r="60" spans="1:6">
       <c r="A60" t="str">
         <f>VLOOKUP(B60,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E60" s="1">
         <v>41307.041666666664</v>
@@ -3802,16 +3802,16 @@
     <row r="61" spans="1:6">
       <c r="A61" t="str">
         <f>VLOOKUP(B61,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E61" s="1">
         <v>41331.6875</v>
@@ -3823,16 +3823,16 @@
     <row r="62" spans="1:6">
       <c r="A62" t="str">
         <f>VLOOKUP(B62,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E62" s="1">
         <v>41359</v>
@@ -3844,16 +3844,16 @@
     <row r="63" spans="1:6">
       <c r="A63" t="str">
         <f>VLOOKUP(B63,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenNilIrrigationFull</v>
+        <v>Lincoln2012NitNilIrrFull</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E63" s="1">
         <v>41359</v>
@@ -3865,16 +3865,16 @@
     <row r="64" spans="1:6">
       <c r="A64" t="str">
         <f>VLOOKUP(B64,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E64" s="1">
         <v>41273.916666666672</v>
@@ -3886,16 +3886,16 @@
     <row r="65" spans="1:6">
       <c r="A65" t="str">
         <f>VLOOKUP(B65,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E65" s="1">
         <v>41279.25</v>
@@ -3907,16 +3907,16 @@
     <row r="66" spans="1:6">
       <c r="A66" t="str">
         <f>VLOOKUP(B66,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B66" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E66" s="1">
         <v>41286.791666666672</v>
@@ -3928,16 +3928,16 @@
     <row r="67" spans="1:6">
       <c r="A67" t="str">
         <f>VLOOKUP(B67,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B67" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E67" s="1">
         <v>41291</v>
@@ -3949,16 +3949,16 @@
     <row r="68" spans="1:6">
       <c r="A68" t="str">
         <f>VLOOKUP(B68,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E68" s="1">
         <v>41298.375</v>
@@ -3970,16 +3970,16 @@
     <row r="69" spans="1:6">
       <c r="A69" t="str">
         <f>VLOOKUP(B69,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B69" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E69" s="1">
         <v>41306.5</v>
@@ -3991,16 +3991,16 @@
     <row r="70" spans="1:6">
       <c r="A70" t="str">
         <f>VLOOKUP(B70,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E70" s="1">
         <v>41324.166666666664</v>
@@ -4012,16 +4012,16 @@
     <row r="71" spans="1:6">
       <c r="A71" t="str">
         <f>VLOOKUP(B71,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenLowIrrigationFull</v>
+        <v>Lincoln2012NitLowIrrFull</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E71" s="1">
         <v>41342.833333333336</v>
@@ -4033,7 +4033,7 @@
     <row r="72" spans="1:6">
       <c r="A72" t="str">
         <f>VLOOKUP(B72,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
@@ -4054,7 +4054,7 @@
     <row r="73" spans="1:6">
       <c r="A73" t="str">
         <f>VLOOKUP(B73,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
@@ -4075,7 +4075,7 @@
     <row r="74" spans="1:6">
       <c r="A74" t="str">
         <f>VLOOKUP(B74,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B74" t="s">
         <v>4</v>
@@ -4096,7 +4096,7 @@
     <row r="75" spans="1:6">
       <c r="A75" t="str">
         <f>VLOOKUP(B75,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B75" t="s">
         <v>4</v>
@@ -4117,7 +4117,7 @@
     <row r="76" spans="1:6">
       <c r="A76" t="str">
         <f>VLOOKUP(B76,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B76" t="s">
         <v>4</v>
@@ -4138,7 +4138,7 @@
     <row r="77" spans="1:6">
       <c r="A77" t="str">
         <f>VLOOKUP(B77,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B77" t="s">
         <v>4</v>
@@ -4159,7 +4159,7 @@
     <row r="78" spans="1:6">
       <c r="A78" t="str">
         <f>VLOOKUP(B78,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B78" t="s">
         <v>4</v>
@@ -4180,7 +4180,7 @@
     <row r="79" spans="1:6">
       <c r="A79" t="str">
         <f>VLOOKUP(B79,Sheet3!C:D,2,FALSE)</f>
-        <v>Lincoln2012NitrogenMedIrrigationFull</v>
+        <v>Lincoln2012NitMedIrrFull</v>
       </c>
       <c r="B79" t="s">
         <v>4</v>
@@ -4213,22 +4213,22 @@
       <selection activeCell="C3" sqref="C3:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:4">
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="3:4">
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="3:4">
@@ -4236,23 +4236,23 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="3:4">
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="3:4">
       <c r="C7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="3:4">
@@ -4260,7 +4260,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>